<commit_message>
UPDATED METRONOME EXCEL FILE
Marc created a list of values that will determine the speed of servo for each BPM setting.

With them I was able to come up with a formula that can give us a more accurate value.

So far I have tested it with the RadioShack Micro servo, the SG90 is still to be tested.

For the SG90 use the column that says, MAX 3000 MIN 1000(speed). This will be included in the source code as a commented out array.
So you can just comment out the other array and use the other one.
</commit_message>
<xml_diff>
--- a/Notes/Metronome_Final.xlsx
+++ b/Notes/Metronome_Final.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trono_000\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6390" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>bpm</t>
   </si>
@@ -27,28 +32,16 @@
     <t>seconds per beat</t>
   </si>
   <si>
-    <t>ts 3/4</t>
+    <t xml:space="preserve"> MAX 2865, MIN 900(speed)</t>
   </si>
   <si>
-    <t>ts 4/4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ts 2/2</t>
-  </si>
-  <si>
-    <t>ts 6/8</t>
-  </si>
-  <si>
-    <t>ts 9/8</t>
-  </si>
-  <si>
-    <t>ts 6/4</t>
+    <t>MAX 3000, MIN 1000(speed)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -96,6 +89,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,25 +422,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="20.125" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="25.625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.875" customWidth="1"/>
+    <col min="7" max="7" width="20.375" customWidth="1"/>
+    <col min="8" max="8" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,61 +448,85 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>40</v>
       </c>
       <c r="B2">
-        <f>1/A2*60</f>
+        <f>ROUNDDOWN(1/A2*60,2)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="C2">
+        <f>ROUNDUP((2865-900)/(((1/A2)*60)/0.02),4)</f>
+        <v>26.2</v>
+      </c>
+      <c r="D2">
+        <f>ROUNDUP((3000-1000)/(((1/A2)*60)/0.02),3)</f>
+        <v>26.667000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>42</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B35" si="0">1/A3*60</f>
-        <v>1.4285714285714284</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <f t="shared" ref="B3:B39" si="0">ROUNDDOWN(1/A3*60,2)</f>
+        <v>1.42</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C39" si="1">ROUNDUP((2865-900)/(((1/A3)*60)/0.02),4)</f>
+        <v>27.51</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D39" si="2">ROUNDUP((3000-1000)/(((1/A3)*60)/0.02),3)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>44</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>1.3636363636363638</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1.36</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>28.82</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>29.334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>46</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>1.3043478260869565</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>1.3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>30.13</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>30.667000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>48</v>
       </c>
@@ -509,266 +534,574 @@
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>31.44</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>32.75</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>33.333999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>34.06</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>34.666999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>54</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>35.369999999999997</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1.03</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>37.99</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>38.666999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>60</v>
       </c>
-      <c r="B7">
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>39.299999999999997</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>63</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>0.95238095238095233</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>41.265000000000001</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>66</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>0.90909090909090917</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>43.23</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>69</v>
       </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>0.86956521739130432</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0.86</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>45.195</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>72</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>0.83333333333333326</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.83</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>47.16</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>76</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>0.78947368421052633</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>49.78</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>50.666999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>80</v>
       </c>
-      <c r="B13">
+      <c r="B17">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>52.4</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>53.333999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>84</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>0.71428571428571419</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>55.02</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>88</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>0.68181818181818188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0.68</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>57.64</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>58.666999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>92</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>0.65217391304347827</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>60.26</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>61.333999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>96</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>62.88</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>100</v>
       </c>
-      <c r="B18">
+      <c r="B22">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>65.5</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>66.667000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>104</v>
       </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>0.57692307692307698</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>68.12</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>69.334000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>108</v>
       </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>0.55555555555555558</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>70.739999999999995</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>112</v>
       </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>0.5357142857142857</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>73.36</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>74.667000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>116</v>
       </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>0.51724137931034486</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>75.98</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>77.334000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>120</v>
       </c>
-      <c r="B23">
+      <c r="B27">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>78.599999999999994</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>126</v>
       </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>0.47619047619047616</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>82.53</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>132</v>
       </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>0.45454545454545459</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>86.46</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>138</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>0.43478260869565216</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>90.39</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>144</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>0.41666666666666663</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0.41</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>94.32</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>152</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>0.39473684210526316</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0.39</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>99.56</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>101.334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>160</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0.37</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>104.8</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>106.667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>168</v>
       </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>0.3571428571428571</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>110.04</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>176</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>0.34090909090909094</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>115.28</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>117.334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>184</v>
       </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>0.32608695652173914</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>120.52</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>122.667</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>192</v>
       </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>0.3125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>0.31</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>125.76</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>200</v>
       </c>
-      <c r="B34">
+      <c r="B38">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35">
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>133.334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>208</v>
       </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>0.28846153846153849</v>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>136.24</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>138.667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>